<commit_message>
SW nochmal korrigiert und Einheiten
</commit_message>
<xml_diff>
--- a/Schrauben/Schrauben/Tabelle-Werte.xlsx
+++ b/Schrauben/Schrauben/Tabelle-Werte.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\Hochsprachenprogrammierung\Sprint\HSP-SoSe-2021\Schrauben\Schrauben\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\Hochsprachenprogrammierung\Sprint\HSP-SoSe-2021\Schrauben\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E5E705-1A34-4A22-8534-659163F58C98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FB309A-D8C6-442B-AD17-02F4CFF43605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="0" windowWidth="28740" windowHeight="15600" xr2:uid="{EC6E8927-7B9C-45F5-9187-D380C00F6962}"/>
   </bookViews>
@@ -584,7 +584,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -615,6 +614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -932,7 +932,7 @@
   <dimension ref="A1:BC66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,14 +947,14 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1091,11 +1091,11 @@
       <c r="B10">
         <v>50</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1146,67 +1146,67 @@
       </c>
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="37" t="s">
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="32"/>
-      <c r="W19" s="32"/>
-      <c r="X19" s="32"/>
-      <c r="Y19" s="32"/>
-      <c r="Z19" s="32"/>
-      <c r="AA19" s="32"/>
-      <c r="AB19" s="32"/>
-      <c r="AC19" s="32"/>
-      <c r="AD19" s="32"/>
-      <c r="AE19" s="32"/>
-      <c r="AF19" s="32"/>
-      <c r="AG19" s="32"/>
-      <c r="AH19" s="32"/>
-      <c r="AI19" s="32"/>
-      <c r="AJ19" s="32"/>
-      <c r="AK19" s="32"/>
-      <c r="AL19" s="32"/>
-      <c r="AM19" s="32"/>
-      <c r="AN19" s="32"/>
-      <c r="AO19" s="32"/>
-      <c r="AP19" s="32"/>
-      <c r="AQ19" s="32"/>
-      <c r="AR19" s="32"/>
-      <c r="AS19" s="32"/>
-      <c r="AT19" s="32"/>
-      <c r="AU19" s="32"/>
-      <c r="AV19" s="38"/>
-      <c r="AW19" s="31" t="s">
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="31"/>
+      <c r="AA19" s="31"/>
+      <c r="AB19" s="31"/>
+      <c r="AC19" s="31"/>
+      <c r="AD19" s="31"/>
+      <c r="AE19" s="31"/>
+      <c r="AF19" s="31"/>
+      <c r="AG19" s="31"/>
+      <c r="AH19" s="31"/>
+      <c r="AI19" s="31"/>
+      <c r="AJ19" s="31"/>
+      <c r="AK19" s="31"/>
+      <c r="AL19" s="31"/>
+      <c r="AM19" s="31"/>
+      <c r="AN19" s="31"/>
+      <c r="AO19" s="31"/>
+      <c r="AP19" s="31"/>
+      <c r="AQ19" s="31"/>
+      <c r="AR19" s="31"/>
+      <c r="AS19" s="31"/>
+      <c r="AT19" s="31"/>
+      <c r="AU19" s="31"/>
+      <c r="AV19" s="37"/>
+      <c r="AW19" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="AX19" s="32"/>
-      <c r="AY19" s="32"/>
-      <c r="AZ19" s="32"/>
-      <c r="BA19" s="32"/>
-      <c r="BB19" s="32"/>
-      <c r="BC19" s="32"/>
+      <c r="AX19" s="31"/>
+      <c r="AY19" s="31"/>
+      <c r="AZ19" s="31"/>
+      <c r="BA19" s="31"/>
+      <c r="BB19" s="31"/>
+      <c r="BC19" s="31"/>
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -5838,7 +5838,7 @@
         <f>IF($B11 = "Sechskant",B34+C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34+Q34+R34+T34+S34+U34+V34+W34+X34+Y34+Z34+AA34+AB34+AC34+AD34+AE34+AF34+AG34+AH34+AI34+AJ34+AK34+AL34+AM34+AN34+AO34+AP34+AQ34+AR34+AS34+AT34+AU34+AV34+AW34+AX34+AY34+AZ34+BA34+BB34+BC34,IF($B11="Zylinderkopf",AW30+AX30+AY30+AZ30+BA30+B30+C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30+Q30+R30+S30+T30+U30+V30+W30+X30+Y30+AA30+Z30+AB30+AC30+AD30+AE30+AF30+AG30+AH30+AI30+AJ30+AK30+AL30+AM30+AN30+AO30+AP30+AQ30+AR30+AS30+AT30+AU30+AV30,IF(B11="Senkkopf",AW39+AX39+AY39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+S39+T39+U39+V39+W39+X39+Y39+Z39+AA39+AB39+AC39+AD39+AE39+AF39+AG39+AH39+AI39+AJ39+AK39+AL39+AM39+AN39+AO39+AP39,"0")))</f>
         <v>65</v>
       </c>
-      <c r="C56" s="26">
+      <c r="C56" s="38">
         <f>D56</f>
         <v>65</v>
       </c>
@@ -5859,7 +5859,7 @@
         <f>IF(B50=0,"0",IF(B16="3.6","180",IF(B16="4.6","240",IF(B16="4.8","320",IF(B16="5.8","400",IF(B16="6.8","480",IF(B16="8.8","640",IF(B16="9.8","720",IF(B16="10.9","900",IF(B16="12.9","1080","0"))))))))))</f>
         <v>240</v>
       </c>
-      <c r="C57" s="30" t="str">
+      <c r="C57" s="29" t="str">
         <f>B57</f>
         <v>240</v>
       </c>
@@ -5874,7 +5874,7 @@
         <f>IF(B50=0,"0",IF(B16="3.6","300",IF(B16="4.6","400",IF(B16="4.8","400",IF(B16="5.8","500",IF(B16="6.8","600",IF(B16="8.8","800",IF(B16="9.8","900",IF(B16="10.9","1000",IF(B16="12.9","1200","0"))))))))))</f>
         <v>400</v>
       </c>
-      <c r="C58" s="30" t="str">
+      <c r="C58" s="29" t="str">
         <f>B58</f>
         <v>400</v>
       </c>
@@ -5888,7 +5888,7 @@
         <f>IF(B8="Stahl",B55*B4*4.25,IF(B8="Aluminium",B55*C4*4.25,IF(B8="Titan",B55*D4*4.25,IF(B8="Messing",B55*E4*4.25,IF(B8="Kupfer",B55*F4*4.25,IF(B8="Bronze",B55*G4*4.25,"0"))))))</f>
         <v>1234.8922951527527</v>
       </c>
-      <c r="C59" s="27">
+      <c r="C59" s="26">
         <f>D59</f>
         <v>1234.8922951527527</v>
       </c>
@@ -5917,7 +5917,7 @@
         <f>MAX(B26:BC26)</f>
         <v>152745.02021569913</v>
       </c>
-      <c r="C60" s="28">
+      <c r="C60" s="27">
         <f>B60</f>
         <v>152745.02021569913</v>
       </c>
@@ -5927,25 +5927,25 @@
       <c r="J62" s="12"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="29"/>
+      <c r="B63" s="28"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="33" t="s">
+      <c r="C65" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="33"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="32"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="33" t="s">
+      <c r="C66" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="D66" s="33"/>
-      <c r="E66" s="33"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="33"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
lokal speichern ja, global nein
</commit_message>
<xml_diff>
--- a/Schrauben/Schrauben/Tabelle-Werte.xlsx
+++ b/Schrauben/Schrauben/Tabelle-Werte.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\Hochsprachenprogrammierung\Sprint\HSP-SoSe-2021\Schrauben\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\Hochsprachenprogrammierung\Sprint\HSP-SoSe-2021\Schrauben\Schrauben\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FB309A-D8C6-442B-AD17-02F4CFF43605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28BBA92-AA1C-4D45-84A4-F054A48DD6A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="0" windowWidth="28740" windowHeight="15600" xr2:uid="{EC6E8927-7B9C-45F5-9187-D380C00F6962}"/>
   </bookViews>
@@ -590,6 +590,7 @@
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,7 +615,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -931,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE13EF1-61C1-43B8-92FA-015A68CF7169}">
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,14 +947,14 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1091,11 +1091,11 @@
       <c r="B10">
         <v>50</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1146,67 +1146,67 @@
       </c>
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="36" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="31"/>
-      <c r="Y19" s="31"/>
-      <c r="Z19" s="31"/>
-      <c r="AA19" s="31"/>
-      <c r="AB19" s="31"/>
-      <c r="AC19" s="31"/>
-      <c r="AD19" s="31"/>
-      <c r="AE19" s="31"/>
-      <c r="AF19" s="31"/>
-      <c r="AG19" s="31"/>
-      <c r="AH19" s="31"/>
-      <c r="AI19" s="31"/>
-      <c r="AJ19" s="31"/>
-      <c r="AK19" s="31"/>
-      <c r="AL19" s="31"/>
-      <c r="AM19" s="31"/>
-      <c r="AN19" s="31"/>
-      <c r="AO19" s="31"/>
-      <c r="AP19" s="31"/>
-      <c r="AQ19" s="31"/>
-      <c r="AR19" s="31"/>
-      <c r="AS19" s="31"/>
-      <c r="AT19" s="31"/>
-      <c r="AU19" s="31"/>
-      <c r="AV19" s="37"/>
-      <c r="AW19" s="30" t="s">
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="32"/>
+      <c r="AA19" s="32"/>
+      <c r="AB19" s="32"/>
+      <c r="AC19" s="32"/>
+      <c r="AD19" s="32"/>
+      <c r="AE19" s="32"/>
+      <c r="AF19" s="32"/>
+      <c r="AG19" s="32"/>
+      <c r="AH19" s="32"/>
+      <c r="AI19" s="32"/>
+      <c r="AJ19" s="32"/>
+      <c r="AK19" s="32"/>
+      <c r="AL19" s="32"/>
+      <c r="AM19" s="32"/>
+      <c r="AN19" s="32"/>
+      <c r="AO19" s="32"/>
+      <c r="AP19" s="32"/>
+      <c r="AQ19" s="32"/>
+      <c r="AR19" s="32"/>
+      <c r="AS19" s="32"/>
+      <c r="AT19" s="32"/>
+      <c r="AU19" s="32"/>
+      <c r="AV19" s="38"/>
+      <c r="AW19" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="AX19" s="31"/>
-      <c r="AY19" s="31"/>
-      <c r="AZ19" s="31"/>
-      <c r="BA19" s="31"/>
-      <c r="BB19" s="31"/>
-      <c r="BC19" s="31"/>
+      <c r="AX19" s="32"/>
+      <c r="AY19" s="32"/>
+      <c r="AZ19" s="32"/>
+      <c r="BA19" s="32"/>
+      <c r="BB19" s="32"/>
+      <c r="BC19" s="32"/>
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -5835,10 +5835,10 @@
         <v>70</v>
       </c>
       <c r="B56" s="10">
-        <f>IF($B11 = "Sechskant",B34+C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34+Q34+R34+T34+S34+U34+V34+W34+X34+Y34+Z34+AA34+AB34+AC34+AD34+AE34+AF34+AG34+AH34+AI34+AJ34+AK34+AL34+AM34+AN34+AO34+AP34+AQ34+AR34+AS34+AT34+AU34+AV34+AW34+AX34+AY34+AZ34+BA34+BB34+BC34,IF($B11="Zylinderkopf",AW30+AX30+AY30+AZ30+BA30+B30+C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30+Q30+R30+S30+T30+U30+V30+W30+X30+Y30+AA30+Z30+AB30+AC30+AD30+AE30+AF30+AG30+AH30+AI30+AJ30+AK30+AL30+AM30+AN30+AO30+AP30+AQ30+AR30+AS30+AT30+AU30+AV30,IF(B11="Senkkopf",AW39+AX39+AY39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+S39+T39+U39+V39+W39+X39+Y39+Z39+AA39+AB39+AC39+AD39+AE39+AF39+AG39+AH39+AI39+AJ39+AK39+AL39+AM39+AN39+AO39+AP39,"0")))</f>
+        <f>IF($B11 = "Sechskant",B34+C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34+Q34+R34+T34+S34+U34+V34+W34+X34+Y34+Z34+AA34+AB34+AC34+AD34+AE34+AF34+AG34+AH34+AI34+AJ34+AK34+AL34+AM34+AN34+AO34+AP34+AQ34+AR34+AS34+AT34+AU34+AV34+AW34+AX34+AY34+AZ34+BA34+BB34+BC34,IF($B11="Zylinderkopf",AW30+AX30+AY30+AZ30+BA30+B30+C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30+Q30+R30+S30+T30+U30+V30+W30+X30+Y30+AA30+Z30+AB30+AC30+AD30+AE30+AF30+AG30+AH30+AI30+AJ30+AK30+AL30+AM30+AN30+AO30+AP30+AQ30+AR30+AS30+AT30+AU30+AV30+BB30+BC30,IF(B11="Senkkopf",AW39+AX39+AY39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+S39+T39+U39+V39+W39+X39+Y39+Z39+AA39+AB39+AC39+AD39+AE39+AF39+AG39+AH39+AI39+AJ39+AK39+AL39+AM39+AN39+AO39+AP39,"0")))</f>
         <v>65</v>
       </c>
-      <c r="C56" s="38">
+      <c r="C56" s="30">
         <f>D56</f>
         <v>65</v>
       </c>
@@ -5930,22 +5930,22 @@
       <c r="B63" s="28"/>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="32"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="32" t="s">
+      <c r="C66" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>